<commit_message>
Fix : Kelas Import
</commit_message>
<xml_diff>
--- a/public/template/template_import_kelas.xlsx
+++ b/public/template/template_import_kelas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ade\js\open-feeder-generator\open-feeder-2\public\bahan_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\TA\siakadppgi\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E658F73D-395C-4BD4-9E50-945B355FE1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFFC6D4-6338-4D28-90B5-D3C6C2560548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{64E36601-E9C9-4122-B907-F1377C20EE8E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{64E36601-E9C9-4122-B907-F1377C20EE8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -750,14 +749,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Semester</t>
   </si>
   <si>
-    <t>Kode Matakuliah</t>
-  </si>
-  <si>
     <t>Nama Matakuliah</t>
   </si>
   <si>
@@ -785,9 +781,6 @@
     <t>Nama Prodi</t>
   </si>
   <si>
-    <t>TI340302</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -816,6 +809,18 @@
   </si>
   <si>
     <t>Sks Simulasi</t>
+  </si>
+  <si>
+    <t>20221</t>
+  </si>
+  <si>
+    <t>AK-001</t>
+  </si>
+  <si>
+    <t>Kode Mata Kuliah</t>
+  </si>
+  <si>
+    <t>1JDLTU</t>
   </si>
 </sst>
 </file>
@@ -1340,109 +1345,109 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C39FCF-0B8A-4E46-8478-6BB73D6B4222}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="9" t="s">
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>20151</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="4">
-        <v>55201</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix : seeder & template
</commit_message>
<xml_diff>
--- a/public/template/template_import_kelas.xlsx
+++ b/public/template/template_import_kelas.xlsx
@@ -1,30 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\TA\siakadppgi\public\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969DBC60-31C6-478E-910A-6C09CFCCBEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{64E36601-E9C9-4122-B907-F1377C20EE8E}"/>
+    <workbookView windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,31 +27,29 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
     <author>S_Denni</author>
     <author>ade surya ramadhani</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{68C88D7D-AA14-419D-B61F-A9C2CE5932D4}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Semester :</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 Contoh : 
@@ -69,32 +62,29 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Warna Merah : Wajib diisi</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{7FCBF85B-8FF9-4DF6-9CF7-91BA07365819}">
+    <comment ref="B1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Kode Matakuliah :</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 Isi dengan Kode Mata Kuliah
@@ -104,9 +94,8 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Warna Merah : Wajib Diisi</t>
         </r>
@@ -114,24 +103,22 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="1" shapeId="0" xr:uid="{4F6F1F89-9D10-48B5-8372-55DA1F13C99D}">
+    <comment ref="C1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Nama Matakuliah :
 </t>
@@ -139,9 +126,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t>Disarankan untuk diisi jika terdapat kode Mata kuliah duplikat. Dianggap duplikat jika Kode Mata kuliah sama tetapi dengan Nama Mata Kuliah yang berbeda</t>
         </r>
@@ -149,24 +135,22 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 Warna Kuning : Diisi jika duplikat.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{2AFEF070-5EDD-477A-B4D9-07D3E76D8005}">
+    <comment ref="D1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Nama Kelas :
 </t>
@@ -174,9 +158,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Isi dengan Nama Kelas. 
 Maksimal 5 karakter</t>
@@ -185,33 +168,30 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 Warna Merah : Wajib Diisi</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{10599706-9E0F-401C-A289-F9E355B92296}">
+    <comment ref="E1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Bahasan :</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 Isi dengan Teks
@@ -221,32 +201,29 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Warna hijau : Boleh Kosong</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{AD68D5E7-83EE-49F0-96D7-8BECC945C4D8}">
+    <comment ref="F1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Tanggal Mulai Efektif : </t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 format : tahun-bulan-tanggal
@@ -256,18 +233,16 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>2017-12-01</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -276,23 +251,21 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Warna Hijau : Boleh Kosong</t>
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="1" shapeId="0" xr:uid="{82D48A3C-5C6F-400E-A513-E2723F4E6FD6}">
+    <comment ref="G1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Tanggal Akhir  Efektif : 
 </t>
@@ -300,9 +273,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>format : tahun-bulan-tanggal
 contoh : 1 Desember 2017 diisi dengan</t>
@@ -311,9 +283,8 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve"> 
 2017-12-01
@@ -321,15 +292,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{D0FD10AD-4B65-403A-8DBA-7E33FD6D1597}">
+    <comment ref="H1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Lingkup Kelas :</t>
         </r>
@@ -337,9 +307,8 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -347,9 +316,8 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Isi dengan angka berikut :</t>
         </r>
@@ -357,9 +325,8 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -367,9 +334,8 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>1 : Internal
 2 : External
@@ -379,9 +345,8 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -389,9 +354,8 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -400,23 +364,21 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Warna Hijau : Boleh Kosong</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{2FCD21C8-21A5-4426-B09E-86E3A622A544}">
+    <comment ref="I1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Mode Kuliah :
 </t>
@@ -424,9 +386,8 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Isi dengan pilihan huruf berikut :
 O : Online
@@ -438,32 +399,29 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Warna Hijau : Boleh Kosong</t>
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{CE9D0A42-4DAF-4219-ACC6-F0A264FE08CF}">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Kode Prodi :</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 Kode Program Studi Dikti
@@ -473,23 +431,21 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Warna Merah : Wajib diisi</t>
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{B12B04A8-675E-4BBC-94E7-F21BF768761E}">
+    <comment ref="K1" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Nama Prodi :
 Tidak wajib diisi, diisi jika ada 2 prodi atau lebih dengan kode prodi dikti sama
@@ -498,9 +454,8 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t>Contoh : 
 12345 : Keperawatan Bandung
@@ -510,24 +465,22 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Rockwell"/>
-            <family val="1"/>
+            <rFont val="Rockwell"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 Warna Kuning : Diisi Jika ada prodi dengan kode sama</t>
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="2" shapeId="0" xr:uid="{61D5E269-4E38-4A6B-8AFF-7AF5729D3436}">
+    <comment ref="L1" authorId="2">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Sks Tatap Muka
 Wajib </t>
@@ -535,9 +488,8 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">diisi jika akan melakukan </t>
         </r>
@@ -545,33 +497,30 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t>update</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve"> kelas kuliah
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="2" shapeId="0" xr:uid="{9B5E8068-ABAE-45F2-A767-46DDFC34AC16}">
+    <comment ref="M1" authorId="2">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Sks Praktek
 </t>
@@ -579,9 +528,8 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -590,18 +538,16 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t>Wajib</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve"> diisi jika akan melakukan </t>
         </r>
@@ -609,42 +555,38 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t>update</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve"> kelas kuliah
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="2" shapeId="0" xr:uid="{5A9E2F8F-B268-4E7C-B9A9-C071EC20CE7C}">
+    <comment ref="N1" authorId="2">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t>Sks Praktek Lapangan</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -653,18 +595,16 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t>Wajib</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve"> diisi jika akan melakukan </t>
         </r>
@@ -672,18 +612,16 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t>update</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve"> kelas kuliah</t>
         </r>
@@ -691,24 +629,22 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="2" shapeId="0" xr:uid="{0545637D-524E-432C-AB76-DDFB3E1F9E53}">
+    <comment ref="O1" authorId="2">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">Sks Simulasi
 Wajib </t>
@@ -716,9 +652,8 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">diisi jika akan melakukan </t>
         </r>
@@ -726,18 +661,16 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t>update</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <charset val="134"/>
           </rPr>
           <t xml:space="preserve"> kelas kuliah
 </t>
@@ -754,6 +687,9 @@
     <t>Semester</t>
   </si>
   <si>
+    <t>Kode Mata Kuliah</t>
+  </si>
+  <si>
     <t>Nama Matakuliah</t>
   </si>
   <si>
@@ -781,6 +717,24 @@
     <t>Nama Prodi</t>
   </si>
   <si>
+    <t>Sks Tatap Muka</t>
+  </si>
+  <si>
+    <t>Sks Praktek</t>
+  </si>
+  <si>
+    <t>Sks Praktek Lapangan</t>
+  </si>
+  <si>
+    <t>Sks Simulasi</t>
+  </si>
+  <si>
+    <t>20221</t>
+  </si>
+  <si>
+    <t>ADA201</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -796,129 +750,264 @@
     <t>M</t>
   </si>
   <si>
+    <t>AK-001</t>
+  </si>
+  <si>
     <t>Nama Prodi (Kota Bandung)</t>
-  </si>
-  <si>
-    <t>Sks Tatap Muka</t>
-  </si>
-  <si>
-    <t>Sks Praktek</t>
-  </si>
-  <si>
-    <t>Sks Praktek Lapangan</t>
-  </si>
-  <si>
-    <t>Sks Simulasi</t>
-  </si>
-  <si>
-    <t>20221</t>
-  </si>
-  <si>
-    <t>AK-001</t>
-  </si>
-  <si>
-    <t>Kode Mata Kuliah</t>
-  </si>
-  <si>
-    <t>1TOLDU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color indexed="63"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Rockwell"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Rockwell"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Rockwell"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Rockwell"/>
-      <family val="1"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Calibri Light"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Calibri Light"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color indexed="63"/>
+      <name val="Helvetica"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <name val="Rockwell"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Rockwell"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Rockwell"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Rockwell"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -955,8 +1044,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -990,57 +1265,341 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF9933"/>
-      <color rgb="FFFFFF66"/>
+      <color rgb="00FF9933"/>
+      <color rgb="00FFFF66"/>
     </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1089,7 +1648,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1122,26 +1681,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1174,23 +1716,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1332,127 +1857,123 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C39FCF-0B8A-4E46-8478-6BB73D6B4222}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" customWidth="1"/>
-    <col min="14" max="14" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.55238095238095" customWidth="1"/>
+    <col min="2" max="2" width="16.4380952380952" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="11.8857142857143" customWidth="1"/>
+    <col min="5" max="5" width="26.4380952380952" customWidth="1"/>
+    <col min="6" max="6" width="20.4380952380952" customWidth="1"/>
+    <col min="7" max="7" width="20.1047619047619" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="12.4380952380952" customWidth="1"/>
+    <col min="10" max="10" width="11.1047619047619" customWidth="1"/>
+    <col min="11" max="11" width="25.8857142857143" customWidth="1"/>
+    <col min="12" max="12" width="19.552380952381" customWidth="1"/>
+    <col min="13" max="13" width="14.8857142857143" customWidth="1"/>
+    <col min="14" max="14" width="21.6666666666667" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" ht="24" customHeight="1" spans="1:15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" ht="15.75" spans="1:11">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="K2" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>